<commit_message>
try commit 291019 0714PM
</commit_message>
<xml_diff>
--- a/BangKeHoach-DoAnCuoiKy.xlsx
+++ b/BangKeHoach-DoAnCuoiKy.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t>DANH SÁCH CÔNG VIỆC</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>5.2 Xây dựng các thành phần GUI</t>
+  </si>
+  <si>
+    <t>3.2 Chạy demo trên GUI</t>
   </si>
 </sst>
 </file>
@@ -535,7 +538,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -543,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W1001"/>
+  <dimension ref="A1:W1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -753,8 +756,13 @@
       <c r="W6" s="8"/>
     </row>
     <row r="7" spans="1:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>19</v>
+      </c>
       <c r="B7" s="9"/>
-      <c r="C7" s="10"/>
+      <c r="C7" s="10" t="s">
+        <v>17</v>
+      </c>
       <c r="D7" s="10"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -775,9 +783,15 @@
       <c r="W7" s="8"/>
     </row>
     <row r="8" spans="1:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
+      <c r="B8" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>17</v>
+      </c>
       <c r="D8" s="10"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="8"/>
@@ -797,14 +811,15 @@
       <c r="W8" s="8"/>
     </row>
     <row r="9" spans="1:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
-        <v>19</v>
+      <c r="B9" s="16" t="s">
+        <v>11</v>
       </c>
-      <c r="B9" s="9"/>
       <c r="C9" s="10" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="10"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="8"/>
@@ -824,8 +839,8 @@
       <c r="W9" s="8"/>
     </row>
     <row r="10" spans="1:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="16" t="s">
-        <v>12</v>
+      <c r="B10" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>17</v>
@@ -834,7 +849,9 @@
       <c r="E10" s="17"/>
       <c r="F10" s="17"/>
       <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
+      <c r="H10" s="7">
+        <v>43765</v>
+      </c>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
@@ -852,12 +869,11 @@
       <c r="W10" s="8"/>
     </row>
     <row r="11" spans="1:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="16" t="s">
-        <v>11</v>
+      <c r="A11" s="16" t="s">
+        <v>9</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>17</v>
-      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="10"/>
       <c r="D11" s="10"/>
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
@@ -880,19 +896,17 @@
       <c r="W11" s="8"/>
     </row>
     <row r="12" spans="1:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="9" t="s">
-        <v>20</v>
+      <c r="B12" s="16" t="s">
+        <v>13</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>17</v>
       </c>
       <c r="D12" s="10"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
       <c r="G12" s="7"/>
-      <c r="H12" s="7">
-        <v>43765</v>
-      </c>
+      <c r="H12" s="7"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
@@ -910,16 +924,15 @@
       <c r="W12" s="8"/>
     </row>
     <row r="13" spans="1:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
-        <v>9</v>
+      <c r="B13" s="16" t="s">
+        <v>24</v>
       </c>
-      <c r="B13" s="9"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="E13" s="17"/>
       <c r="F13" s="17"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
@@ -937,13 +950,16 @@
       <c r="W13" s="8"/>
     </row>
     <row r="14" spans="1:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="16" t="s">
-        <v>13</v>
+      <c r="A14" s="16" t="s">
+        <v>10</v>
       </c>
+      <c r="B14" s="9"/>
       <c r="C14" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="10"/>
+      <c r="D14" s="10" t="s">
+        <v>17</v>
+      </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
@@ -965,13 +981,8 @@
       <c r="W14" s="8"/>
     </row>
     <row r="15" spans="1:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
-        <v>10</v>
-      </c>
       <c r="B15" s="9"/>
-      <c r="C15" s="10" t="s">
-        <v>17</v>
-      </c>
+      <c r="C15" s="10"/>
       <c r="D15" s="10"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
@@ -994,6 +1005,9 @@
       <c r="W15" s="8"/>
     </row>
     <row r="16" spans="1:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>14</v>
+      </c>
       <c r="B16" s="9"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
@@ -1018,16 +1032,17 @@
       <c r="W16" s="8"/>
     </row>
     <row r="17" spans="1:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
-        <v>14</v>
+      <c r="B17" s="9" t="s">
+        <v>22</v>
       </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="10"/>
+      <c r="C17" s="10" t="s">
+        <v>17</v>
+      </c>
       <c r="D17" s="10"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
@@ -1045,17 +1060,17 @@
       <c r="W17" s="8"/>
     </row>
     <row r="18" spans="1:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="9" t="s">
-        <v>22</v>
+      <c r="B18" s="16" t="s">
+        <v>23</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>17</v>
       </c>
       <c r="D18" s="10"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
@@ -1073,9 +1088,10 @@
       <c r="W18" s="8"/>
     </row>
     <row r="19" spans="1:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="16" t="s">
-        <v>23</v>
+      <c r="A19" s="16" t="s">
+        <v>15</v>
       </c>
+      <c r="B19" s="9"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
       <c r="E19" s="7"/>
@@ -1099,9 +1115,6 @@
       <c r="W19" s="8"/>
     </row>
     <row r="20" spans="1:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="16" t="s">
-        <v>15</v>
-      </c>
       <c r="B20" s="9"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
@@ -1245,38 +1258,34 @@
       <c r="V25" s="8"/>
       <c r="W25" s="8"/>
     </row>
-    <row r="26" spans="1:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="9"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8"/>
-      <c r="P26" s="8"/>
-      <c r="Q26" s="8"/>
-      <c r="R26" s="8"/>
-      <c r="S26" s="8"/>
-      <c r="T26" s="8"/>
-      <c r="U26" s="8"/>
-      <c r="V26" s="8"/>
-      <c r="W26" s="8"/>
-    </row>
-    <row r="27" spans="1:23" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="13"/>
+      <c r="O26" s="13"/>
+      <c r="P26" s="13"/>
+      <c r="Q26" s="13"/>
+      <c r="R26" s="13"/>
+      <c r="S26" s="13"/>
+    </row>
+    <row r="27" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
       <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
+      <c r="H27" s="14"/>
       <c r="I27" s="13"/>
       <c r="J27" s="13"/>
       <c r="K27" s="13"/>
@@ -1296,7 +1305,7 @@
       <c r="E28" s="12"/>
       <c r="F28" s="12"/>
       <c r="G28" s="12"/>
-      <c r="H28" s="14"/>
+      <c r="H28" s="12"/>
       <c r="I28" s="13"/>
       <c r="J28" s="13"/>
       <c r="K28" s="13"/>
@@ -20748,26 +20757,6 @@
       <c r="Q1000" s="13"/>
       <c r="R1000" s="13"/>
       <c r="S1000" s="13"/>
-    </row>
-    <row r="1001" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1001" s="1"/>
-      <c r="C1001" s="11"/>
-      <c r="D1001" s="11"/>
-      <c r="E1001" s="12"/>
-      <c r="F1001" s="12"/>
-      <c r="G1001" s="12"/>
-      <c r="H1001" s="12"/>
-      <c r="I1001" s="13"/>
-      <c r="J1001" s="13"/>
-      <c r="K1001" s="13"/>
-      <c r="L1001" s="13"/>
-      <c r="M1001" s="13"/>
-      <c r="N1001" s="13"/>
-      <c r="O1001" s="13"/>
-      <c r="P1001" s="13"/>
-      <c r="Q1001" s="13"/>
-      <c r="R1001" s="13"/>
-      <c r="S1001" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
try commit Bao cao
</commit_message>
<xml_diff>
--- a/BangKeHoach-DoAnCuoiKy.xlsx
+++ b/BangKeHoach-DoAnCuoiKy.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
   <si>
     <t>DANH SÁCH CÔNG VIỆC</t>
   </si>
@@ -90,15 +90,6 @@
   </si>
   <si>
     <t>3.2 Chạy demo trên GUI</t>
-  </si>
-  <si>
-    <t>Nút xóa 1 phần tử cuối của biểu thức</t>
-  </si>
-  <si>
-    <t>Nút clear textbox</t>
-  </si>
-  <si>
-    <t>Nút lưu kết quả vào file</t>
   </si>
 </sst>
 </file>
@@ -547,7 +538,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -557,8 +548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -797,10 +788,18 @@
       <c r="D8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
+      <c r="E8" s="17">
+        <v>43740</v>
+      </c>
+      <c r="F8" s="17">
+        <v>43740</v>
+      </c>
+      <c r="G8" s="7">
+        <v>43753</v>
+      </c>
+      <c r="H8" s="17">
+        <v>43753</v>
+      </c>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
@@ -915,7 +914,9 @@
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
+      <c r="H12" s="17">
+        <v>43765</v>
+      </c>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
@@ -941,7 +942,9 @@
       <c r="E13" s="17"/>
       <c r="F13" s="17"/>
       <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
+      <c r="H13" s="17">
+        <v>43765</v>
+      </c>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
@@ -1052,8 +1055,12 @@
       </c>
       <c r="E17" s="17"/>
       <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
+      <c r="G17" s="17">
+        <v>43733</v>
+      </c>
+      <c r="H17" s="17">
+        <v>43734</v>
+      </c>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
@@ -1082,8 +1089,12 @@
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
+      <c r="G18" s="17">
+        <v>43733</v>
+      </c>
+      <c r="H18" s="7">
+        <v>43734</v>
+      </c>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
@@ -1128,12 +1139,8 @@
       <c r="W19" s="8"/>
     </row>
     <row r="20" spans="1:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>17</v>
-      </c>
+      <c r="B20" s="9"/>
+      <c r="C20" s="10"/>
       <c r="D20" s="10"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
@@ -1156,13 +1163,9 @@
       <c r="W20" s="8"/>
     </row>
     <row r="21" spans="1:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="9" t="s">
-        <v>26</v>
-      </c>
+      <c r="B21" s="9"/>
       <c r="C21" s="10"/>
-      <c r="D21" s="10" t="s">
-        <v>17</v>
-      </c>
+      <c r="D21" s="10"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
@@ -1184,12 +1187,8 @@
       <c r="W21" s="8"/>
     </row>
     <row r="22" spans="1:23" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>17</v>
-      </c>
+      <c r="B22" s="9"/>
+      <c r="C22" s="10"/>
       <c r="D22" s="10"/>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>

</xml_diff>